<commit_message>
Changed the sample property code from 1000 to 1234
To avoid confusion with accounts starting with 1XXX
</commit_message>
<xml_diff>
--- a/Example General Ledger Report.xlsx
+++ b/Example General Ledger Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TBGL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\TBGL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996BCCD0-E085-4B26-903C-AB99137157F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33356EF3-DAC3-41DE-BAA1-6624B9F0AC62}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C47A58B0-6DCD-4985-A6ED-82075218723A}"/>
   </bookViews>
@@ -60,9 +60,6 @@
     <t>Location:</t>
   </si>
   <si>
-    <t>1000--Example Property</t>
-  </si>
-  <si>
     <t>Posted Dt.</t>
   </si>
   <si>
@@ -340,6 +337,9 @@
   </si>
   <si>
     <t>INTEREST</t>
+  </si>
+  <si>
+    <t>1234--Example Property</t>
   </si>
 </sst>
 </file>
@@ -719,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{948034C5-9B45-497A-8264-A89B44D940DD}">
   <dimension ref="A1:AB120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,47 +780,47 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="K7" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K8" s="4">
         <v>353170.47</v>
@@ -834,16 +834,16 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9">
+        <v>1000</v>
+      </c>
+      <c r="H9" t="s">
         <v>24</v>
-      </c>
-      <c r="F9">
-        <v>1000</v>
-      </c>
-      <c r="H9" t="s">
-        <v>25</v>
       </c>
       <c r="J9" s="4">
         <v>801</v>
@@ -861,16 +861,16 @@
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
         <v>39</v>
       </c>
-      <c r="D10" t="s">
-        <v>40</v>
-      </c>
       <c r="F10">
         <v>1000</v>
       </c>
       <c r="H10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I10" s="4">
         <v>324</v>
@@ -888,16 +888,16 @@
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11">
         <v>1000</v>
       </c>
       <c r="H11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I11" s="4">
         <v>397</v>
@@ -915,16 +915,16 @@
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12">
         <v>1000</v>
       </c>
       <c r="H12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I12" s="4">
         <v>1680</v>
@@ -942,16 +942,16 @@
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F13">
         <v>1000</v>
       </c>
       <c r="H13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I13" s="4">
         <v>129</v>
@@ -969,16 +969,16 @@
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F14">
         <v>1000</v>
       </c>
       <c r="H14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J14" s="4">
         <v>81243.83</v>
@@ -996,16 +996,16 @@
         <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F15">
         <v>1000</v>
       </c>
       <c r="H15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I15" s="4">
         <v>1045</v>
@@ -1017,22 +1017,22 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F16">
         <v>1000</v>
       </c>
       <c r="H16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I16" s="4">
         <v>970</v>
@@ -1044,22 +1044,22 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F17">
         <v>1000</v>
       </c>
       <c r="H17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I17" s="4">
         <v>7817</v>
@@ -1071,22 +1071,22 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F18">
         <v>1000</v>
       </c>
       <c r="H18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I18" s="4">
         <v>1550</v>
@@ -1098,22 +1098,22 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F19">
         <v>1000</v>
       </c>
       <c r="H19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I19" s="4">
         <v>896.86</v>
@@ -1125,22 +1125,22 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F20">
         <v>1000</v>
       </c>
       <c r="H20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J20" s="4">
         <v>4172.32</v>
@@ -1158,16 +1158,16 @@
         <v>9</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F21">
         <v>1000</v>
       </c>
       <c r="H21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J21" s="4">
         <v>19261.55</v>
@@ -1179,7 +1179,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I22" s="5">
         <f>SUM(I8:I21)</f>
@@ -1196,7 +1196,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K25" s="4">
         <v>127094.71</v>
@@ -1210,13 +1210,13 @@
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F26">
         <v>1000</v>
       </c>
       <c r="H26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I26" s="4">
         <v>449.81</v>
@@ -1228,7 +1228,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I27" s="5">
         <f>SUM(I25:I26)</f>
@@ -1245,7 +1245,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K30" s="4">
         <v>15.81</v>
@@ -1253,7 +1253,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I31" s="5">
         <f>SUM(I30:I30)</f>
@@ -1270,7 +1270,7 @@
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K34" s="4">
         <v>30601.17</v>
@@ -1284,13 +1284,13 @@
         <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F35">
         <v>1000</v>
       </c>
       <c r="H35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I35" s="4">
         <v>20172.169999999998</v>
@@ -1308,13 +1308,13 @@
         <v>9</v>
       </c>
       <c r="D36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F36">
         <v>1000</v>
       </c>
       <c r="H36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I36" s="4">
         <v>58.49</v>
@@ -1326,7 +1326,7 @@
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I37" s="5">
         <f>SUM(I34:I36)</f>
@@ -1365,7 +1365,7 @@
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K40" s="4">
         <v>55486.95</v>
@@ -1385,13 +1385,13 @@
         <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F41">
         <v>1000</v>
       </c>
       <c r="H41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I41" s="4">
         <v>12836.45</v>
@@ -1415,13 +1415,13 @@
         <v>9</v>
       </c>
       <c r="D42" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F42">
         <v>1000</v>
       </c>
       <c r="H42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I42" s="4">
         <v>58.49</v>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I43" s="5">
         <f>SUM(I40:I42)</f>
@@ -1450,7 +1450,7 @@
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K46" s="4">
         <v>188570.72</v>
@@ -1464,13 +1464,13 @@
         <v>7</v>
       </c>
       <c r="D47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F47">
         <v>1000</v>
       </c>
       <c r="H47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I47" s="4">
         <v>4750</v>
@@ -1488,13 +1488,13 @@
         <v>9</v>
       </c>
       <c r="D48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F48">
         <v>1000</v>
       </c>
       <c r="H48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I48" s="4">
         <v>243.32</v>
@@ -1506,7 +1506,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I49" s="5">
         <f>SUM(I46:I48)</f>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K52" s="4">
         <v>3933</v>
@@ -1537,13 +1537,13 @@
         <v>7</v>
       </c>
       <c r="D53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F53">
         <v>1000</v>
       </c>
       <c r="H53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I53" s="4">
         <v>1891.1</v>
@@ -1561,13 +1561,13 @@
         <v>9</v>
       </c>
       <c r="D54" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F54">
         <v>1000</v>
       </c>
       <c r="H54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I54" s="4">
         <v>6.83</v>
@@ -1579,7 +1579,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I55" s="5">
         <f>SUM(I52:I54)</f>
@@ -1596,7 +1596,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K58" s="4">
         <v>163315.18</v>
@@ -1610,13 +1610,13 @@
         <v>9</v>
       </c>
       <c r="D59" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F59">
         <v>1000</v>
       </c>
       <c r="H59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I59" s="4">
         <v>206.66</v>
@@ -1628,7 +1628,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I60" s="5">
         <f>SUM(I58:I59)</f>
@@ -1645,7 +1645,7 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K63" s="4">
         <v>826402.73</v>
@@ -1659,13 +1659,13 @@
         <v>9</v>
       </c>
       <c r="D64" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F64">
         <v>1000</v>
       </c>
       <c r="H64" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I64" s="4">
         <v>0.19</v>
@@ -1683,13 +1683,13 @@
         <v>9</v>
       </c>
       <c r="D65" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F65">
         <v>1000</v>
       </c>
       <c r="H65" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I65" s="4">
         <v>0.01</v>
@@ -1701,7 +1701,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I66" s="5">
         <f>SUM(I63:I65)</f>
@@ -1718,7 +1718,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K69" s="4">
         <v>225913.05</v>
@@ -1732,13 +1732,13 @@
         <v>9</v>
       </c>
       <c r="D70" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F70">
         <v>1000</v>
       </c>
       <c r="H70" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I70" s="4">
         <v>728.79</v>
@@ -1756,13 +1756,13 @@
         <v>9</v>
       </c>
       <c r="D71" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F71">
         <v>1000</v>
       </c>
       <c r="H71" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I71" s="4">
         <v>3558.5</v>
@@ -1774,7 +1774,7 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I72" s="5">
         <f>SUM(I69:I71)</f>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K75" s="4">
         <v>131419.19</v>
@@ -1805,16 +1805,16 @@
         <v>7</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D76" t="s">
+        <v>88</v>
+      </c>
+      <c r="F76">
+        <v>1000</v>
+      </c>
+      <c r="H76" t="s">
         <v>89</v>
-      </c>
-      <c r="F76">
-        <v>1000</v>
-      </c>
-      <c r="H76" t="s">
-        <v>90</v>
       </c>
       <c r="I76" s="4">
         <v>142389.85999999999</v>
@@ -1832,16 +1832,16 @@
         <v>7</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D77" t="s">
+        <v>88</v>
+      </c>
+      <c r="F77">
+        <v>1000</v>
+      </c>
+      <c r="H77" t="s">
         <v>89</v>
-      </c>
-      <c r="F77">
-        <v>1000</v>
-      </c>
-      <c r="H77" t="s">
-        <v>90</v>
       </c>
       <c r="J77" s="4">
         <v>8399.9699999999993</v>
@@ -1859,16 +1859,16 @@
         <v>7</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D78" t="s">
+        <v>88</v>
+      </c>
+      <c r="F78">
+        <v>1000</v>
+      </c>
+      <c r="H78" t="s">
         <v>89</v>
-      </c>
-      <c r="F78">
-        <v>1000</v>
-      </c>
-      <c r="H78" t="s">
-        <v>90</v>
       </c>
       <c r="J78" s="4">
         <v>447</v>
@@ -1886,16 +1886,16 @@
         <v>7</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D79" t="s">
+        <v>88</v>
+      </c>
+      <c r="F79">
+        <v>1000</v>
+      </c>
+      <c r="H79" t="s">
         <v>89</v>
-      </c>
-      <c r="F79">
-        <v>1000</v>
-      </c>
-      <c r="H79" t="s">
-        <v>90</v>
       </c>
       <c r="J79" s="4">
         <v>2489.34</v>
@@ -1913,16 +1913,16 @@
         <v>7</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D80" t="s">
+        <v>88</v>
+      </c>
+      <c r="F80">
+        <v>1000</v>
+      </c>
+      <c r="H80" t="s">
         <v>89</v>
-      </c>
-      <c r="F80">
-        <v>1000</v>
-      </c>
-      <c r="H80" t="s">
-        <v>90</v>
       </c>
       <c r="J80" s="4">
         <v>99.45</v>
@@ -1937,19 +1937,19 @@
         <v>7</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D81" t="s">
+        <v>88</v>
+      </c>
+      <c r="F81">
+        <v>1000</v>
+      </c>
+      <c r="H81" t="s">
         <v>89</v>
-      </c>
-      <c r="F81">
-        <v>1000</v>
-      </c>
-      <c r="H81" t="s">
-        <v>90</v>
       </c>
       <c r="J81" s="4">
         <v>4695</v>
@@ -1964,16 +1964,16 @@
         <v>7</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D82" t="s">
+        <v>88</v>
+      </c>
+      <c r="F82">
+        <v>1000</v>
+      </c>
+      <c r="H82" t="s">
         <v>89</v>
-      </c>
-      <c r="F82">
-        <v>1000</v>
-      </c>
-      <c r="H82" t="s">
-        <v>90</v>
       </c>
       <c r="J82" s="4">
         <v>1849</v>
@@ -1985,19 +1985,19 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D83" t="s">
+        <v>88</v>
+      </c>
+      <c r="F83">
+        <v>1000</v>
+      </c>
+      <c r="H83" t="s">
         <v>89</v>
-      </c>
-      <c r="F83">
-        <v>1000</v>
-      </c>
-      <c r="H83" t="s">
-        <v>90</v>
       </c>
       <c r="I83" s="4">
         <v>3.66</v>
@@ -2009,19 +2009,19 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D84" t="s">
+        <v>88</v>
+      </c>
+      <c r="F84">
+        <v>1000</v>
+      </c>
+      <c r="H84" t="s">
         <v>89</v>
-      </c>
-      <c r="F84">
-        <v>1000</v>
-      </c>
-      <c r="H84" t="s">
-        <v>90</v>
       </c>
       <c r="J84" s="4">
         <v>1844</v>
@@ -2033,22 +2033,22 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D85" t="s">
+        <v>88</v>
+      </c>
+      <c r="F85">
+        <v>1000</v>
+      </c>
+      <c r="H85" t="s">
         <v>89</v>
-      </c>
-      <c r="F85">
-        <v>1000</v>
-      </c>
-      <c r="H85" t="s">
-        <v>90</v>
       </c>
       <c r="J85" s="4">
         <v>18049.990000000002</v>
@@ -2060,22 +2060,22 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D86" t="s">
+        <v>88</v>
+      </c>
+      <c r="F86">
+        <v>1000</v>
+      </c>
+      <c r="H86" t="s">
         <v>89</v>
-      </c>
-      <c r="F86">
-        <v>1000</v>
-      </c>
-      <c r="H86" t="s">
-        <v>90</v>
       </c>
       <c r="J86" s="4">
         <v>8774.83</v>
@@ -2087,22 +2087,22 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C87" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D87" t="s">
         <v>88</v>
       </c>
-      <c r="D87" t="s">
+      <c r="F87">
+        <v>1000</v>
+      </c>
+      <c r="H87" t="s">
         <v>89</v>
-      </c>
-      <c r="F87">
-        <v>1000</v>
-      </c>
-      <c r="H87" t="s">
-        <v>90</v>
       </c>
       <c r="I87" s="4">
         <v>165</v>
@@ -2120,16 +2120,16 @@
         <v>9</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D88" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F88">
         <v>1000</v>
       </c>
       <c r="H88" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J88" s="4">
         <v>92757.27</v>
@@ -2141,7 +2141,7 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I89" s="5">
         <f>SUM(I75:I88)</f>
@@ -2158,7 +2158,7 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K92" s="4">
         <v>5026.26</v>
@@ -2172,16 +2172,16 @@
         <v>7</v>
       </c>
       <c r="C93" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D93" t="s">
         <v>93</v>
       </c>
-      <c r="D93" t="s">
-        <v>94</v>
-      </c>
       <c r="F93">
         <v>1000</v>
       </c>
       <c r="H93" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J93" s="4">
         <v>166.26</v>
@@ -2199,16 +2199,16 @@
         <v>7</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D94" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F94">
         <v>1000</v>
       </c>
       <c r="H94" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J94" s="4">
         <v>3815</v>
@@ -2226,16 +2226,16 @@
         <v>7</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D95" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F95">
         <v>1000</v>
       </c>
       <c r="H95" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J95" s="4">
         <v>1045</v>
@@ -2253,13 +2253,13 @@
         <v>7</v>
       </c>
       <c r="D96" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F96">
         <v>1000</v>
       </c>
       <c r="H96" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I96" s="4">
         <v>117.24</v>
@@ -2277,13 +2277,13 @@
         <v>7</v>
       </c>
       <c r="D97" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F97">
         <v>1000</v>
       </c>
       <c r="H97" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I97" s="4">
         <v>173.92</v>
@@ -2298,7 +2298,7 @@
         <v>7</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D98" t="s">
         <v>5</v>
@@ -2307,7 +2307,7 @@
         <v>1000</v>
       </c>
       <c r="H98" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I98" s="4">
         <v>2365</v>
@@ -2319,7 +2319,7 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I99" s="5">
         <f>SUM(I92:I98)</f>
@@ -2336,7 +2336,7 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K102" s="4">
         <v>-76395.62</v>
@@ -2350,16 +2350,16 @@
         <v>7</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D103" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F103">
         <v>1000</v>
       </c>
       <c r="H103" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J103" s="4">
         <v>324</v>
@@ -2377,16 +2377,16 @@
         <v>7</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D104" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F104">
         <v>1000</v>
       </c>
       <c r="H104" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J104" s="4">
         <v>397</v>
@@ -2404,16 +2404,16 @@
         <v>7</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D105" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F105">
         <v>1000</v>
       </c>
       <c r="H105" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J105" s="4">
         <v>1682</v>
@@ -2431,16 +2431,16 @@
         <v>7</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D106" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F106">
         <v>1000</v>
       </c>
       <c r="H106" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J106" s="4">
         <v>129</v>
@@ -2458,16 +2458,16 @@
         <v>7</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D107" t="s">
+        <v>88</v>
+      </c>
+      <c r="F107">
+        <v>1000</v>
+      </c>
+      <c r="H107" t="s">
         <v>89</v>
-      </c>
-      <c r="F107">
-        <v>1000</v>
-      </c>
-      <c r="H107" t="s">
-        <v>90</v>
       </c>
       <c r="I107" s="4">
         <v>46256.800000000003</v>
@@ -2482,19 +2482,19 @@
         <v>7</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D108" t="s">
+        <v>88</v>
+      </c>
+      <c r="F108">
+        <v>1000</v>
+      </c>
+      <c r="H108" t="s">
         <v>89</v>
-      </c>
-      <c r="F108">
-        <v>1000</v>
-      </c>
-      <c r="H108" t="s">
-        <v>90</v>
       </c>
       <c r="I108" s="4">
         <v>8399.9699999999993</v>
@@ -2509,16 +2509,16 @@
         <v>7</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D109" t="s">
+        <v>88</v>
+      </c>
+      <c r="F109">
+        <v>1000</v>
+      </c>
+      <c r="H109" t="s">
         <v>89</v>
-      </c>
-      <c r="F109">
-        <v>1000</v>
-      </c>
-      <c r="H109" t="s">
-        <v>90</v>
       </c>
       <c r="I109" s="4">
         <v>447</v>
@@ -2530,19 +2530,19 @@
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D110" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F110">
         <v>1000</v>
       </c>
       <c r="H110" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J110" s="4">
         <v>970</v>
@@ -2554,19 +2554,19 @@
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D111" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F111">
         <v>1000</v>
       </c>
       <c r="H111" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J111" s="4">
         <v>7817</v>
@@ -2578,22 +2578,22 @@
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D112" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F112">
         <v>1000</v>
       </c>
       <c r="H112" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J112" s="4">
         <v>1550</v>
@@ -2605,22 +2605,22 @@
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D113" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F113">
         <v>1000</v>
       </c>
       <c r="H113" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J113" s="4">
         <v>896.86</v>
@@ -2632,22 +2632,22 @@
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C114" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D114" t="s">
         <v>88</v>
       </c>
-      <c r="D114" t="s">
+      <c r="F114">
+        <v>1000</v>
+      </c>
+      <c r="H114" t="s">
         <v>89</v>
-      </c>
-      <c r="F114">
-        <v>1000</v>
-      </c>
-      <c r="H114" t="s">
-        <v>90</v>
       </c>
       <c r="I114" s="4">
         <v>2494.83</v>
@@ -2665,16 +2665,16 @@
         <v>9</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D115" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F115">
         <v>1000</v>
       </c>
       <c r="H115" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J115" s="4">
         <v>28499.02</v>
@@ -2686,7 +2686,7 @@
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I116" s="5">
         <f>SUM(I102:I115)</f>
@@ -2703,7 +2703,7 @@
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K118" s="6">
         <v>-2034553.62</v>
@@ -2717,13 +2717,13 @@
         <v>9</v>
       </c>
       <c r="D119" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F119">
         <v>1000</v>
       </c>
       <c r="H119" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I119" s="6">
         <v>29568.44</v>
@@ -2735,7 +2735,7 @@
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I120" s="5">
         <f>SUM(I118:I119)</f>

</xml_diff>